<commit_message>
feat: update test write 2 rows in go-generate-excel
</commit_message>
<xml_diff>
--- a/go-generate-excel/excel/gen_16092023.xlsx
+++ b/go-generate-excel/excel/gen_16092023.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Date Transaction</t>
   </si>
@@ -30,7 +30,7 @@
     <t>Total</t>
   </si>
   <si>
-    <t>1 transactions</t>
+    <t>2 transactions</t>
   </si>
   <si>
     <t>No.1</t>
@@ -58,6 +58,18 @@
   </si>
   <si>
     <t>example detail</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>10:00:00</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>example detail 2</t>
   </si>
 </sst>
 </file>
@@ -103,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -115,6 +127,24 @@
       <right style=""/>
       <top style=""/>
       <bottom style=""/>
+    </border>
+    <border>
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style=""/>
+    </border>
+    <border>
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+    </border>
+    <border>
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style=""/>
+      <bottom style="hair"/>
     </border>
     <border>
       <left style="thin">
@@ -131,23 +161,32 @@
       </bottom>
     </border>
   </borders>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="0" applyNumberFormat="1" applyProtection="0" borderId="1" fillId="0" fontId="0" numFmtId="166" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="2" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="0" applyNumberFormat="1" applyProtection="0" borderId="3" fillId="0" fontId="0" numFmtId="166" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="3" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="1" applyFont="1" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="1" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="1" applyFont="1" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="1" numFmtId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -487,7 +526,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -495,9 +534,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="9.14" customWidth="true"/>
-    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="9.14" customWidth="true"/>
-    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="9.14" customWidth="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.14" customWidth="true"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.08" customWidth="true"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.14" customWidth="true"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.55" customWidth="true"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="9.14" customWidth="true"/>
   </cols>
@@ -509,57 +548,77 @@
       <c r="B1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4"/>
     <row r="5">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="8" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>